<commit_message>
added git commands to embedded_interview doc
</commit_message>
<xml_diff>
--- a/DailyUpdate_Sheet.xlsx
+++ b/DailyUpdate_Sheet.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -117,6 +117,16 @@
   </si>
   <si>
     <t>18.07.2015 (doc file)</t>
+  </si>
+  <si>
+    <t>copied git commands to
+embedded interview doc</t>
+  </si>
+  <si>
+    <t>fa03bbce022b8909f4d14a627e7aa1915a782d29</t>
+  </si>
+  <si>
+    <t>check Embedded interview doc</t>
   </si>
 </sst>
 </file>
@@ -124,7 +134,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-409]h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -209,7 +219,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -509,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -600,6 +610,29 @@
       </c>
       <c r="G3" s="5" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="30">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>